<commit_message>
modification des conditions sur les bénéficiaires
</commit_message>
<xml_diff>
--- a/new_payments_v2.xlsx
+++ b/new_payments_v2.xlsx
@@ -17,33 +17,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
-  <si>
-    <t>Expéditeur</t>
-  </si>
-  <si>
-    <t>Bénéficiaire</t>
-  </si>
-  <si>
-    <t>Montant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date d’exécution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Détails des frais</t>
-  </si>
-  <si>
-    <t>Urgence</t>
-  </si>
-  <si>
-    <t>Libellé</t>
-  </si>
-  <si>
-    <t>Commentaire</t>
-  </si>
-  <si>
-    <t>Titulaire</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+  <si>
+    <t>Sender</t>
+  </si>
+  <si>
+    <t>Recipient</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Execution date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fees option</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
   <si>
     <t>IBAN</t>
@@ -61,19 +64,22 @@
     <t>22108000006912</t>
   </si>
   <si>
+    <t>USD</t>
+  </si>
+  <si>
     <t>client</t>
   </si>
   <si>
-    <t>BE17914001921521</t>
-  </si>
-  <si>
-    <t>b44126a0e90b4d4</t>
-  </si>
-  <si>
-    <t>RS35160005010008573607</t>
-  </si>
-  <si>
-    <t>bénéficiaire</t>
+    <t>314b065159e8e9c</t>
+  </si>
+  <si>
+    <t>RS35155000000000563774</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>recipient</t>
   </si>
   <si>
     <t>BE12914005042392</t>
@@ -85,7 +91,7 @@
     <t>10943409100132</t>
   </si>
   <si>
-    <t>partagé</t>
+    <t>share</t>
   </si>
 </sst>
 </file>
@@ -95,7 +101,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd;@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.000000"/>
       <color theme="1"/>
@@ -114,17 +120,21 @@
     </font>
     <font>
       <sz val="10.000000"/>
-      <name val="Nimbus Roman"/>
+      <name val="Asana"/>
     </font>
     <font>
       <b/>
       <sz val="13.000000"/>
       <color theme="0" tint="0"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
+      <name val="Asana"/>
+    </font>
+    <font>
+      <sz val="10.000000"/>
+      <color theme="1"/>
+      <name val="Asana"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,18 +158,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF6F9D4"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF729FCF"/>
-        <bgColor indexed="55"/>
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor theme="8" tint="0.59999389629810485"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -186,15 +190,6 @@
       <diagonal style="none"/>
     </border>
     <border>
-      <left style="none"/>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
       <left style="thin">
         <color theme="1"/>
       </left>
@@ -221,7 +216,7 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
     <xf fontId="2" fillId="2" borderId="1" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -231,52 +226,60 @@
     <xf fontId="3" fillId="0" borderId="2" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="4" fillId="3" borderId="0" numFmtId="49" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="4" fillId="3" borderId="0" numFmtId="49" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="4" fillId="4" borderId="3" numFmtId="49" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="4" fillId="4" borderId="3" numFmtId="164" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="3" fillId="5" borderId="3" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="4" fillId="0" borderId="3" numFmtId="49" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="4" fillId="0" borderId="3" numFmtId="164" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="5" fillId="0" borderId="3" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="5" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="5" fillId="0" borderId="3" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
     <xf fontId="3" fillId="0" borderId="3" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="3" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="3" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="3" fillId="0" borderId="3" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="4" fillId="3" borderId="1" numFmtId="49" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="4" fillId="4" borderId="1" numFmtId="49" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="4" fillId="4" borderId="1" numFmtId="164" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="3" fillId="5" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="3" fillId="6" borderId="4" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right"/>
+    <xf fontId="3" fillId="0" borderId="3" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="0">
@@ -727,248 +730,243 @@
   <cols>
     <col bestFit="1" customWidth="1" min="1" max="1" style="2" width="17.57421875"/>
     <col bestFit="1" customWidth="1" min="2" max="2" style="3" width="17.8515625"/>
-    <col customWidth="1" min="3" max="3" style="4" width="18.539999999999999"/>
-    <col customWidth="1" min="4" max="4" style="4" width="22.68"/>
-    <col customWidth="0" min="5" max="5" style="1" width="11.529999999999999"/>
-    <col bestFit="1" customWidth="1" min="6" max="6" style="5" width="21.28125"/>
-    <col bestFit="1" customWidth="1" min="7" max="7" style="1" width="20.421875"/>
-    <col bestFit="1" customWidth="0" min="8" max="8" style="1" width="11.00390625"/>
-    <col customWidth="0" min="9" max="9" style="1" width="11.529999999999999"/>
-    <col bestFit="1" customWidth="1" min="10" max="10" style="6" width="16.8515625"/>
-    <col customWidth="0" min="11" max="16384" style="1" width="11.529999999999999"/>
+    <col customWidth="1" min="3" max="3" style="1" width="18.539999999999999"/>
+    <col bestFit="1" customWidth="1" min="4" max="4" style="1" width="24.23046875"/>
+    <col bestFit="1" customWidth="0" min="5" max="5" style="1" width="10.140625"/>
+    <col customWidth="0" min="6" max="6" style="1" width="10.140625"/>
+    <col bestFit="1" customWidth="1" min="7" max="7" style="4" width="19.421875"/>
+    <col bestFit="1" customWidth="1" min="8" max="8" style="1" width="20.421875"/>
+    <col bestFit="1" customWidth="0" min="9" max="9" style="1" width="9.140625"/>
+    <col bestFit="1" customWidth="0" min="10" max="10" style="1" width="13.421875"/>
+    <col bestFit="1" customWidth="1" min="11" max="11" style="3" width="15.57421875"/>
+    <col customWidth="0" min="12" max="16384" style="1" width="11.529999999999999"/>
   </cols>
   <sheetData>
     <row r="1" ht="38.399999999999999" customHeight="1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="8" t="s">
+      <c r="D1" s="5"/>
+      <c r="E1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="7" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" s="10" customFormat="1" ht="15">
-      <c r="A2" s="11" t="s">
+      <c r="K1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="11" t="s">
+    </row>
+    <row r="2" s="9" customFormat="1" ht="17.25">
+      <c r="A2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="11" t="s">
+      <c r="B2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-    </row>
-    <row r="3" s="10" customFormat="1" ht="12.800000000000001">
-      <c r="A3" s="12" t="s">
+      <c r="D2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+    </row>
+    <row r="3" s="9" customFormat="1" ht="13.5">
+      <c r="A3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="B3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="C3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="13">
+      <c r="D3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="14">
-        <v>45723</v>
-      </c>
-      <c r="G3" s="13" t="s">
+      <c r="E3" s="14">
         <v>14</v>
       </c>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-    </row>
-    <row r="4" s="10" customFormat="1" ht="12.800000000000001">
-      <c r="A4" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="12" t="s">
+      <c r="F3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="G3" s="15">
+        <v>45728</v>
+      </c>
+      <c r="H3" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+    </row>
+    <row r="4" s="9" customFormat="1" ht="13.5">
+      <c r="A4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="13">
+      <c r="D4" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="14">
         <v>25</v>
       </c>
-      <c r="F4" s="14">
-        <v>45724</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-    </row>
-    <row r="5" s="10" customFormat="1" ht="12.800000000000001">
-      <c r="A5" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="12" t="s">
+      <c r="F4" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="G4" s="15">
+        <v>45744</v>
+      </c>
+      <c r="H4" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+    </row>
+    <row r="5" s="9" customFormat="1" ht="13.5">
+      <c r="A5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="13">
+      <c r="C5" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="14">
         <v>9</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="15">
         <v>45725</v>
       </c>
-      <c r="G5" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-    </row>
-    <row r="6" s="10" customFormat="1" ht="12.800000000000001">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="13"/>
+      <c r="H5" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+    </row>
+    <row r="6" s="9" customFormat="1" ht="12.800000000000001">
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="14"/>
       <c r="F6" s="14"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-    </row>
-    <row r="7" s="10" customFormat="1" ht="12.800000000000001">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="13">
-        <v>23</v>
-      </c>
+      <c r="G6" s="15"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+    </row>
+    <row r="7" s="9" customFormat="1" ht="12.800000000000001">
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="14"/>
       <c r="F7" s="14"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-    </row>
-    <row r="8" s="10" customFormat="1" ht="12.800000000000001">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-    </row>
-    <row r="9" s="10" customFormat="1" ht="12.800000000000001">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-    </row>
-    <row r="10" s="10" customFormat="1" ht="12.800000000000001">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-    </row>
-    <row r="11" s="10" customFormat="1" ht="12.800000000000001">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-    </row>
-    <row r="12" s="10" customFormat="1" ht="12.800000000000001">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-    </row>
-    <row r="13" s="10" customFormat="1" ht="12.800000000000001">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-    </row>
-    <row r="18" ht="12.800000000000001">
-      <c r="D18" s="16"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+    </row>
+    <row r="8" s="3" customFormat="1" ht="12.75">
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+    </row>
+    <row r="9" ht="12.75">
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+    </row>
+    <row r="10" ht="12.75">
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" ht="12.75">
+      <c r="A11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" ht="12.800000000000001">
+      <c r="D12" s="18"/>
+    </row>
+    <row r="13" ht="12.75">
+      <c r="K13" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:E2"/>
@@ -977,6 +975,7 @@
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins left="0.78750000000000009" right="0.78750000000000009" top="1.05277777777778" bottom="1.05277777777778" header="0.78750000000000009" footer="0.78750000000000009"/>

</xml_diff>

<commit_message>
switch language in web app
</commit_message>
<xml_diff>
--- a/new_payments_v2.xlsx
+++ b/new_payments_v2.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Sender</t>
   </si>
@@ -58,40 +58,19 @@
     <t>BE39914001921319</t>
   </si>
   <si>
-    <t>622f987fda43500</t>
-  </si>
-  <si>
-    <t>22108000006912</t>
-  </si>
-  <si>
-    <t>USD</t>
+    <t>314b065159e8e9c</t>
+  </si>
+  <si>
+    <t>RS35155000000000563774</t>
+  </si>
+  <si>
+    <t>EUR</t>
   </si>
   <si>
     <t>client</t>
   </si>
   <si>
-    <t>314b065159e8e9c</t>
-  </si>
-  <si>
-    <t>RS35155000000000563774</t>
-  </si>
-  <si>
-    <t>EUR</t>
-  </si>
-  <si>
     <t>recipient</t>
-  </si>
-  <si>
-    <t>BE12914005042392</t>
-  </si>
-  <si>
-    <t>d64dcdf43fa8dbb</t>
-  </si>
-  <si>
-    <t>10943409100132</t>
-  </si>
-  <si>
-    <t>share</t>
   </si>
 </sst>
 </file>
@@ -216,7 +195,7 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
     <xf fontId="2" fillId="2" borderId="1" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -226,14 +205,7 @@
     <xf fontId="3" fillId="0" borderId="2" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="3" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="4" fillId="3" borderId="0" numFmtId="49" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="4" fillId="3" borderId="0" numFmtId="49" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
@@ -729,163 +701,153 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75"/>
   <cols>
     <col bestFit="1" customWidth="1" min="1" max="1" style="2" width="17.57421875"/>
-    <col bestFit="1" customWidth="1" min="2" max="2" style="3" width="17.8515625"/>
+    <col bestFit="1" customWidth="1" min="2" max="2" style="1" width="17.8515625"/>
     <col customWidth="1" min="3" max="3" style="1" width="18.539999999999999"/>
     <col bestFit="1" customWidth="1" min="4" max="4" style="1" width="24.23046875"/>
     <col bestFit="1" customWidth="0" min="5" max="5" style="1" width="10.140625"/>
     <col customWidth="0" min="6" max="6" style="1" width="10.140625"/>
-    <col bestFit="1" customWidth="1" min="7" max="7" style="4" width="19.421875"/>
+    <col bestFit="1" customWidth="1" min="7" max="7" style="3" width="19.421875"/>
     <col bestFit="1" customWidth="1" min="8" max="8" style="1" width="20.421875"/>
     <col bestFit="1" customWidth="0" min="9" max="9" style="1" width="9.140625"/>
     <col bestFit="1" customWidth="0" min="10" max="10" style="1" width="13.421875"/>
-    <col bestFit="1" customWidth="1" min="11" max="11" style="3" width="15.57421875"/>
+    <col bestFit="1" customWidth="1" min="11" max="11" style="1" width="15.57421875"/>
     <col customWidth="0" min="12" max="16384" style="1" width="11.529999999999999"/>
   </cols>
   <sheetData>
     <row r="1" ht="38.399999999999999" customHeight="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="7" t="s">
+      <c r="D1" s="4"/>
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" s="9" customFormat="1" ht="17.25">
-      <c r="A2" s="10" t="s">
+    <row r="2" s="7" customFormat="1" ht="13.5">
+      <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-    </row>
-    <row r="3" s="9" customFormat="1" ht="13.5">
-      <c r="A3" s="13" t="s">
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+    </row>
+    <row r="3" s="7" customFormat="1" ht="13.5">
+      <c r="A3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="12">
         <v>14</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="15">
+      <c r="G3" s="13">
         <v>45728</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-    </row>
-    <row r="4" s="9" customFormat="1" ht="13.5">
-      <c r="A4" s="13" t="s">
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+    </row>
+    <row r="4" s="7" customFormat="1" ht="13.5">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="12">
+        <v>25</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="13">
+        <v>45744</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+    </row>
+    <row r="5" s="7" customFormat="1" ht="13.5">
+      <c r="A5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="14">
-        <v>25</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="15">
-        <v>45744</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-    </row>
-    <row r="5" s="9" customFormat="1" ht="13.5">
-      <c r="A5" s="13" t="s">
+      <c r="C5" s="11"/>
+      <c r="D5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="12">
         <v>11</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="14">
-        <v>9</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="15">
-        <v>45725</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-    </row>
-    <row r="6" s="9" customFormat="1" ht="12.800000000000001">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+    </row>
+    <row r="6" s="1" customFormat="1" ht="12.75">
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
       <c r="G6" s="15"/>
@@ -894,11 +856,11 @@
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
     </row>
-    <row r="7" s="9" customFormat="1" ht="12.800000000000001">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
+    <row r="7" ht="12.75">
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
       <c r="G7" s="15"/>
@@ -907,63 +869,47 @@
       <c r="J7" s="14"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" s="3" customFormat="1" ht="12.75">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
+    <row r="8" ht="12.75">
+      <c r="A8" s="2"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
     </row>
     <row r="9" ht="12.75">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-    </row>
-    <row r="10" ht="12.75">
+      <c r="A9" s="2"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" ht="12.800000000000001">
       <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
+      <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="D10" s="16"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="4"/>
+      <c r="G10" s="3"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="3"/>
+      <c r="K10" s="1"/>
     </row>
     <row r="11" ht="12.75">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="3"/>
-    </row>
-    <row r="12" ht="12.800000000000001">
-      <c r="D12" s="18"/>
-    </row>
-    <row r="13" ht="12.75">
-      <c r="K13" s="3"/>
+      <c r="K11" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
app web fonctionne et sdk structré en classe
</commit_message>
<xml_diff>
--- a/new_payments_v2.xlsx
+++ b/new_payments_v2.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Sender</t>
   </si>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t>44</t>
-  </si>
-  <si>
-    <t>OTTO</t>
   </si>
 </sst>
 </file>
@@ -1023,10 +1020,8 @@
       <c r="J7" s="5"/>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" ht="13.5">
-      <c r="A8" s="2" t="s">
-        <v>27</v>
-      </c>
+    <row r="8" ht="12.75">
+      <c r="A8" s="2"/>
       <c r="K8" s="7"/>
     </row>
   </sheetData>

</xml_diff>